<commit_message>
Slow Test Finish. Ready to use jk program
</commit_message>
<xml_diff>
--- a/documents/controll.xlsx
+++ b/documents/controll.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\THINPAD2\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\THU\2016Autumn\CPU\THINPAD2\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13620" windowHeight="5208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13620" windowHeight="5205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="184">
   <si>
     <t>ADDIU</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -696,63 +696,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OE&lt;=0,FINISH&lt;=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAControl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC=JR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTHING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001,RAC=00000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEMX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEMY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAC=MEMY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAC=MEMX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OE&lt;=0,FINISH&lt;=0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RAControl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC=JR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>00000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOTHING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001,RAC=00000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEMX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEMY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RAC=MEMY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RAC=MEMX</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1094,28 +1098,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1"/>
-    <col min="4" max="4" width="17.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="11" width="9" style="1"/>
-    <col min="12" max="12" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="9" style="1"/>
-    <col min="16" max="16" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="9" style="1"/>
-    <col min="20" max="20" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.875" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -1143,11 +1147,11 @@
       </c>
       <c r="N1" s="3"/>
       <c r="O1" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1173,13 +1177,13 @@
         <v>105</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1206,13 +1210,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>109</v>
@@ -1227,7 +1231,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1253,9 +1257,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>109</v>
@@ -1277,7 +1281,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
@@ -1318,7 +1322,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="K9" s="3"/>
       <c r="L9" s="1" t="s">
         <v>89</v>
@@ -1330,7 +1334,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
@@ -1365,7 +1369,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="K12" s="3"/>
       <c r="L12" s="1" t="s">
         <v>165</v>
@@ -1377,7 +1381,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="D14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="K15" s="3"/>
       <c r="L15" s="1" t="s">
         <v>95</v>
@@ -1436,7 +1440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="D17" s="1" t="s">
         <v>53</v>
       </c>
@@ -1471,7 +1475,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="K18" s="3"/>
       <c r="L18" s="1" t="s">
         <v>95</v>
@@ -1483,7 +1487,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1503,7 +1507,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="O21" s="1" t="s">
         <v>158</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="O23" s="1" t="s">
         <v>160</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -1564,7 +1568,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="O25" s="1" t="s">
         <v>162</v>
       </c>
@@ -1572,7 +1576,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1580,21 +1584,21 @@
         <v>18</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P26" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="O27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O27" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -1610,12 +1614,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="D31" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1623,12 +1627,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D34" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -1636,12 +1640,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D37" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -1649,12 +1653,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D40" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -1665,10 +1669,10 @@
         <v>33</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1676,12 +1680,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E44" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E45" s="1" t="s">
         <v>36</v>
       </c>
@@ -1689,7 +1693,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E46" s="1" t="s">
         <v>163</v>
       </c>
@@ -1697,7 +1701,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1708,10 +1712,10 @@
         <v>33</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E48" s="1" t="s">
         <v>34</v>
       </c>
@@ -1719,12 +1723,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E49" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E50" s="1" t="s">
         <v>36</v>
       </c>
@@ -1732,7 +1736,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E51" s="1" t="s">
         <v>108</v>
       </c>
@@ -1740,7 +1744,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>41</v>
       </c>
@@ -1748,12 +1752,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D53" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -1761,12 +1765,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
@@ -1774,12 +1778,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D59" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>47</v>
       </c>
@@ -1787,12 +1791,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D62" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>49</v>
       </c>
@@ -1800,12 +1804,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D65" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>51</v>
       </c>
@@ -1813,12 +1817,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D68" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>55</v>
       </c>
@@ -1826,7 +1830,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
@@ -1834,12 +1838,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D73" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>59</v>
       </c>
@@ -1847,12 +1851,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D76" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>62</v>
       </c>
@@ -1860,12 +1864,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D79" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>65</v>
       </c>
@@ -1873,12 +1877,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D82" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>67</v>
       </c>
@@ -1886,12 +1890,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D85" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>70</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D88" s="1" t="s">
         <v>74</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E89" s="1" t="s">
         <v>75</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E90" s="1" t="s">
         <v>76</v>
       </c>
@@ -1926,15 +1930,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E91" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F91" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>77</v>
       </c>
@@ -1945,7 +1949,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="D93" s="1" t="s">
         <v>74</v>
       </c>
@@ -1953,7 +1957,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E94" s="1" t="s">
         <v>75</v>
       </c>
@@ -1961,7 +1965,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E95" s="1" t="s">
         <v>76</v>
       </c>
@@ -1969,25 +1973,25 @@
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="E96" s="1" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K9"/>
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="K13:K15"/>
     <mergeCell ref="K16:K18"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="K8:K9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>